<commit_message>
hpa_HielprikAlgemeen gestript en werkend
</commit_message>
<xml_diff>
--- a/src/main/resources/nhs-dmn/OriginelenVoorBusiness/ActiesGeneriekOrigineel.xlsx
+++ b/src/main/resources/nhs-dmn/OriginelenVoorBusiness/ActiesGeneriekOrigineel.xlsx
@@ -8,25 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\han\git\rivm\nhs\dmn\nhs-business\src\main\resources\nhs-dmn\OriginelenVoorBusiness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3609C9-3BBA-47EC-ACD8-7148E2B3EB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B54359-74E8-49A8-A7FF-0F7B0A9E68E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32010" yWindow="-915" windowWidth="28800" windowHeight="13050" tabRatio="834" activeTab="6" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" activeTab="6" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
   </bookViews>
   <sheets>
     <sheet name="Lijstjes" sheetId="7" r:id="rId1"/>
     <sheet name="Actiecode" sheetId="10" r:id="rId2"/>
     <sheet name="ConclusieEA" sheetId="28" r:id="rId3"/>
-    <sheet name="ActieBT" sheetId="15" r:id="rId4"/>
+    <sheet name="Status BT" sheetId="15" r:id="rId4"/>
     <sheet name="isTweedeHielprik" sheetId="24" r:id="rId5"/>
     <sheet name="isPrematuur" sheetId="13" r:id="rId6"/>
     <sheet name="isTeVroegGeprikt" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ActieBT!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Actiecode!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Actiecode!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ConclusieEA!$A$1:$B$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">isPrematuur!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">isTweedeHielprik!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Status BT'!$A$1:$D$1</definedName>
     <definedName name="ActieBTwaarden">Lijstjes!$C$2:$C$6</definedName>
     <definedName name="ActieCodeWaarden">Lijstjes!$D$2:$D$10</definedName>
     <definedName name="AfnameTermijnVeld">Lijstjes!$L$2:$L$4</definedName>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="130">
   <si>
     <t>Actiecode</t>
   </si>
@@ -343,9 +343,6 @@
     <t>HPS.isTeVroegGeprikt</t>
   </si>
   <si>
-    <t>BTnavraagNodig</t>
-  </si>
-  <si>
     <t>"AFW"</t>
   </si>
   <si>
@@ -448,9 +445,6 @@
     <t>ConclusieEA</t>
   </si>
   <si>
-    <t>ActieBT</t>
-  </si>
-  <si>
     <t>"Navraag nodig"</t>
   </si>
   <si>
@@ -461,6 +455,9 @@
   </si>
   <si>
     <t>VoldoendeTijdVerstrekenBT</t>
+  </si>
+  <si>
+    <t>Status BT</t>
   </si>
 </sst>
 </file>
@@ -644,10 +641,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -983,25 +976,25 @@
         <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D1" t="s">
         <v>14</v>
       </c>
       <c r="E1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" t="s">
         <v>100</v>
       </c>
-      <c r="F1" t="s">
-        <v>101</v>
-      </c>
       <c r="G1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" t="s">
         <v>110</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>111</v>
-      </c>
-      <c r="I1" t="s">
-        <v>112</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
@@ -1051,22 +1044,22 @@
         <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I2" t="s">
         <v>39</v>
@@ -1119,22 +1112,22 @@
         <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I3" t="s">
         <v>41</v>
@@ -1190,22 +1183,22 @@
         <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J4" t="s">
         <v>50</v>
@@ -1258,7 +1251,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
@@ -1267,13 +1260,13 @@
         <v>20</v>
       </c>
       <c r="G5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" t="s">
+        <v>112</v>
+      </c>
+      <c r="I5" t="s">
         <v>114</v>
-      </c>
-      <c r="H5" t="s">
-        <v>113</v>
-      </c>
-      <c r="I5" t="s">
-        <v>115</v>
       </c>
       <c r="J5" t="s">
         <v>54</v>
@@ -1314,7 +1307,7 @@
         <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E6" t="s">
         <v>52</v>
@@ -1358,7 +1351,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G7" t="s">
         <v>20</v>
@@ -1390,7 +1383,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K8" t="s">
         <v>48</v>
@@ -1410,7 +1403,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K9" t="s">
         <v>51</v>
@@ -1424,7 +1417,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K10" t="s">
         <v>50</v>
@@ -1459,43 +1452,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{510755D5-C225-4368-836B-774EA8447DE4}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>39</v>
       </c>
@@ -1508,14 +1497,11 @@
       <c r="D2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>40</v>
       </c>
@@ -1528,74 +1514,62 @@
       <c r="D3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="E3" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>46</v>
       </c>
@@ -1608,14 +1582,11 @@
       <c r="D7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>47</v>
       </c>
@@ -1628,14 +1599,11 @@
       <c r="D8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -1648,14 +1616,11 @@
       <c r="D9" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>41</v>
       </c>
@@ -1666,16 +1631,13 @@
         <v>52</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>41</v>
       </c>
@@ -1686,93 +1648,82 @@
         <v>52</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5"/>
+      <c r="E19" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{510755D5-C225-4368-836B-774EA8447DE4}"/>
+  <autoFilter ref="A1:E1" xr:uid="{510755D5-C225-4368-836B-774EA8447DE4}"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{5CEB2CE4-8CFA-4134-81D2-BFB2D7298F51}">
       <formula1>Interpretatie</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:E1048576" xr:uid="{B7860D93-30E1-4DF2-B242-9FCAB1ADD29B}">
-      <formula1>JaNeeVeld</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{D35B422F-4F69-4E7A-A279-CD20110817B3}">
       <formula1>ActieBTwaarden</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{2BCA14A3-EA85-45D8-B73B-618CEDD0987B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{2BCA14A3-EA85-45D8-B73B-618CEDD0987B}">
       <formula1>ActieCodeWaarden</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D1048576" xr:uid="{B7860D93-30E1-4DF2-B242-9FCAB1ADD29B}">
+      <formula1>JaNeeVeld</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1798,87 +1749,87 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1949,13 +1900,13 @@
         <v>78</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2006,7 +1957,7 @@
         <v>52</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F4" t="s">
         <v>52</v>
@@ -2043,7 +1994,7 @@
         <v>83</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2060,7 +2011,7 @@
         <v>84</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2077,7 +2028,7 @@
         <v>85</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2094,7 +2045,7 @@
         <v>86</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2111,7 +2062,7 @@
         <v>87</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>